<commit_message>
Pulled in documentation changes
</commit_message>
<xml_diff>
--- a/man/completed sheets/2015-10-26/Maurice_Corriettetimesheet261015.xlsx
+++ b/man/completed sheets/2015-10-26/Maurice_Corriettetimesheet261015.xlsx
@@ -474,7 +474,7 @@
       <pane xSplit="8" ySplit="2" topLeftCell="I3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,11 +510,11 @@
       </c>
       <c r="G1" s="4" t="str">
         <f>"Total hours accounted this week: " &amp;TEXT(I1, "hh:mm")</f>
-        <v>Total hours accounted this week: 17:00</v>
+        <v>Total hours accounted this week: 12:00</v>
       </c>
       <c r="I1" s="6">
         <f>SUM(F3:F100)</f>
-        <v>0.70833333333333337</v>
+        <v>0.5</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -568,7 +568,7 @@
         <v>42305</v>
       </c>
       <c r="F3" s="11">
-        <v>0.1875</v>
+        <v>0.14583333333333334</v>
       </c>
       <c r="G3" s="9"/>
       <c r="H3" s="9"/>
@@ -590,7 +590,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="11">
-        <v>0.52083333333333337</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>

</xml_diff>